<commit_message>
Atualizações no PDV: ajustes no app.py, templates e deploy para Railway
</commit_message>
<xml_diff>
--- a/data/produtos.xlsx
+++ b/data/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,234 +436,92 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>codigo_barras</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>nome</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>tipo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>preco_venda</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>estoque</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>perecivel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>validade</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>preco_custo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>margem_venda</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>preco_venda</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>estoque</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>perecivel</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>validade</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cebola KG</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>peso</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+          <t>Alface Und</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
       <c r="F2" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="G2" t="n">
-        <v>15.9</v>
+        <v>14</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Hortaliças</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>hortifruti</t>
+          <t>nao</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>7501030683414</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Queijo ralado Kinino 40g</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>unidade</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>5.99</v>
-      </c>
-      <c r="G3" t="n">
-        <v>9</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>mercearia</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Banana Nanica KG</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>peso</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>5.99</v>
-      </c>
-      <c r="G4" t="n">
-        <v>18</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>hortifruti</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TOMATE KG</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>peso</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="G5" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>hortifruti</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ALFACE UND</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>unidade</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="G6" t="n">
-        <v>100</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>hortifruti</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>